<commit_message>
Updating strHisCl1 plots to include a comparison between histamine+ iL3s and unstimulated wild-type iL3s
</commit_message>
<xml_diff>
--- a/Neural Imaging/R Plotting/Data/Tax4HisCl1_R_Import.xlsx
+++ b/Neural Imaging/R Plotting/Data/Tax4HisCl1_R_Import.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Box Sync/Lab_Hallem/Astra/Writing/Bryant et al 20xx/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrasb/Documents/RStudio/Bryant_et_al_2021/Neural Imaging/R Plotting/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8287AD54-544B-464F-BE53-7726189A3406}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9316B7-2EE4-664F-B60C-C4C4E884834E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="4020" windowWidth="27640" windowHeight="16940" xr2:uid="{BDAE310E-8061-A349-B10C-027791E49373}"/>
+    <workbookView xWindow="36560" yWindow="2600" windowWidth="27640" windowHeight="16940" xr2:uid="{BDAE310E-8061-A349-B10C-027791E49373}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="15">
   <si>
     <t>Experiment</t>
   </si>
@@ -68,12 +68,15 @@
   <si>
     <t>NoCas9</t>
   </si>
+  <si>
+    <t>Unstimulated</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -93,6 +96,15 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,10 +127,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,16 +447,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78EE2EAE-83F1-B841-9ABC-A60199FA4338}">
-  <dimension ref="A1:F193"/>
+  <dimension ref="A1:F208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="E162" sqref="E162"/>
+    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="A202" sqref="A202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -4305,6 +4320,261 @@
         <v>6.8211375842371316E-2</v>
       </c>
     </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>14</v>
+      </c>
+      <c r="B194" t="s">
+        <v>6</v>
+      </c>
+      <c r="C194" t="s">
+        <v>14</v>
+      </c>
+      <c r="E194" s="3">
+        <v>5.8945999999999996</v>
+      </c>
+      <c r="F194" s="4">
+        <v>0.25886999999999999</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>14</v>
+      </c>
+      <c r="B195" t="s">
+        <v>6</v>
+      </c>
+      <c r="C195" t="s">
+        <v>14</v>
+      </c>
+      <c r="E195" s="3">
+        <v>11.372999999999999</v>
+      </c>
+      <c r="F195" s="4">
+        <v>0.1404</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>14</v>
+      </c>
+      <c r="B196" t="s">
+        <v>6</v>
+      </c>
+      <c r="C196" t="s">
+        <v>14</v>
+      </c>
+      <c r="E196" s="3">
+        <v>6.7539999999999996</v>
+      </c>
+      <c r="F196" s="4">
+        <v>0.14377999999999999</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>14</v>
+      </c>
+      <c r="B197" t="s">
+        <v>6</v>
+      </c>
+      <c r="C197" t="s">
+        <v>14</v>
+      </c>
+      <c r="E197" s="3">
+        <v>4.4067999999999996</v>
+      </c>
+      <c r="F197" s="4">
+        <v>0.14842</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>14</v>
+      </c>
+      <c r="B198" t="s">
+        <v>6</v>
+      </c>
+      <c r="C198" t="s">
+        <v>14</v>
+      </c>
+      <c r="E198" s="3">
+        <v>6.7714999999999996</v>
+      </c>
+      <c r="F198" s="4">
+        <v>0.14435000000000001</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>14</v>
+      </c>
+      <c r="B199" t="s">
+        <v>6</v>
+      </c>
+      <c r="C199" t="s">
+        <v>14</v>
+      </c>
+      <c r="E199" s="3">
+        <v>6.9790000000000001</v>
+      </c>
+      <c r="F199" s="4">
+        <v>0.19669</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>14</v>
+      </c>
+      <c r="B200" t="s">
+        <v>6</v>
+      </c>
+      <c r="C200" t="s">
+        <v>14</v>
+      </c>
+      <c r="E200" s="3">
+        <v>4.3243999999999998</v>
+      </c>
+      <c r="F200" s="4">
+        <v>9.4409000000000007E-2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>14</v>
+      </c>
+      <c r="B201" t="s">
+        <v>6</v>
+      </c>
+      <c r="C201" t="s">
+        <v>14</v>
+      </c>
+      <c r="E201" s="3">
+        <v>4.9255000000000004</v>
+      </c>
+      <c r="F201" s="4">
+        <v>0.21004999999999999</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>14</v>
+      </c>
+      <c r="B202" t="s">
+        <v>6</v>
+      </c>
+      <c r="C202" t="s">
+        <v>14</v>
+      </c>
+      <c r="E202" s="3">
+        <v>7.2979000000000003</v>
+      </c>
+      <c r="F202" s="4">
+        <v>5.5652E-2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>14</v>
+      </c>
+      <c r="B203" t="s">
+        <v>6</v>
+      </c>
+      <c r="C203" t="s">
+        <v>14</v>
+      </c>
+      <c r="E203" s="3">
+        <v>8.4199000000000002</v>
+      </c>
+      <c r="F203" s="4">
+        <v>0.12307999999999999</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>14</v>
+      </c>
+      <c r="B204" t="s">
+        <v>6</v>
+      </c>
+      <c r="C204" t="s">
+        <v>14</v>
+      </c>
+      <c r="E204" s="3">
+        <v>7.5479000000000003</v>
+      </c>
+      <c r="F204" s="4">
+        <v>0.26830999999999999</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>14</v>
+      </c>
+      <c r="B205" t="s">
+        <v>6</v>
+      </c>
+      <c r="C205" t="s">
+        <v>14</v>
+      </c>
+      <c r="E205" s="3">
+        <v>9.7294999999999998</v>
+      </c>
+      <c r="F205" s="4">
+        <v>0.22291</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>14</v>
+      </c>
+      <c r="B206" t="s">
+        <v>6</v>
+      </c>
+      <c r="C206" t="s">
+        <v>14</v>
+      </c>
+      <c r="E206" s="3">
+        <v>6.2157</v>
+      </c>
+      <c r="F206" s="4">
+        <v>0.28038000000000002</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>14</v>
+      </c>
+      <c r="B207" t="s">
+        <v>6</v>
+      </c>
+      <c r="C207" t="s">
+        <v>14</v>
+      </c>
+      <c r="E207" s="3">
+        <v>18.492999999999999</v>
+      </c>
+      <c r="F207" s="4">
+        <v>0.17806</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>14</v>
+      </c>
+      <c r="B208" t="s">
+        <v>6</v>
+      </c>
+      <c r="C208" t="s">
+        <v>14</v>
+      </c>
+      <c r="E208" s="3">
+        <v>12.8</v>
+      </c>
+      <c r="F208" s="4">
+        <v>6.7672999999999997E-2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>